<commit_message>
Fixed values, analysis matrix added
</commit_message>
<xml_diff>
--- a/CRIq_new_dataworksheet.xlsx
+++ b/CRIq_new_dataworksheet.xlsx
@@ -926,6 +926,9 @@
       <c r="AC4">
         <v>243</v>
       </c>
+      <c r="AF4">
+        <v>96</v>
+      </c>
       <c r="AG4">
         <v>117</v>
       </c>
@@ -1027,6 +1030,9 @@
       <c r="AC5">
         <v>307</v>
       </c>
+      <c r="AF5">
+        <v>98</v>
+      </c>
       <c r="AG5">
         <v>108</v>
       </c>
@@ -1544,6 +1550,9 @@
       <c r="AC10">
         <v>117</v>
       </c>
+      <c r="AF10">
+        <v>89</v>
+      </c>
       <c r="AG10">
         <v>86</v>
       </c>
@@ -1645,6 +1654,9 @@
       <c r="AC11">
         <v>65</v>
       </c>
+      <c r="AF11">
+        <v>91</v>
+      </c>
       <c r="AG11">
         <v>113</v>
       </c>
@@ -1746,6 +1758,9 @@
       <c r="AC12">
         <v>272</v>
       </c>
+      <c r="AF12">
+        <v>122</v>
+      </c>
       <c r="AG12">
         <v>127</v>
       </c>
@@ -2783,6 +2798,9 @@
       <c r="AC22">
         <v>349</v>
       </c>
+      <c r="AF22">
+        <v>133</v>
+      </c>
       <c r="AG22">
         <v>135</v>
       </c>
@@ -3404,6 +3422,9 @@
       <c r="AC28">
         <v>80</v>
       </c>
+      <c r="AF28">
+        <v>115</v>
+      </c>
       <c r="AG28">
         <v>123</v>
       </c>
@@ -4129,6 +4150,9 @@
       <c r="AC35">
         <v>210</v>
       </c>
+      <c r="AF35">
+        <v>121</v>
+      </c>
       <c r="AG35">
         <v>119</v>
       </c>
@@ -4854,6 +4878,9 @@
       <c r="AC42">
         <v>300</v>
       </c>
+      <c r="AF42">
+        <v>124</v>
+      </c>
       <c r="AG42">
         <v>134</v>
       </c>
@@ -5053,6 +5080,9 @@
       <c r="AC44">
         <v>45</v>
       </c>
+      <c r="AF44">
+        <v>99</v>
+      </c>
       <c r="AG44">
         <v>107</v>
       </c>
@@ -5736,6 +5766,9 @@
       <c r="AC51">
         <v>392</v>
       </c>
+      <c r="AF51">
+        <v>130</v>
+      </c>
       <c r="AG51">
         <v>136</v>
       </c>
@@ -6027,6 +6060,9 @@
       <c r="AC54">
         <v>523</v>
       </c>
+      <c r="AF54">
+        <v>136</v>
+      </c>
       <c r="AG54">
         <v>123</v>
       </c>
@@ -6416,6 +6452,9 @@
       <c r="AC58">
         <v>316</v>
       </c>
+      <c r="AF58">
+        <v>110</v>
+      </c>
       <c r="AG58">
         <v>106</v>
       </c>
@@ -6995,6 +7034,9 @@
       <c r="AC64">
         <v>330</v>
       </c>
+      <c r="AF64">
+        <v>72</v>
+      </c>
       <c r="AG64">
         <v>19</v>
       </c>
@@ -7090,6 +7132,9 @@
       <c r="AC65">
         <v>199</v>
       </c>
+      <c r="AF65">
+        <v>76</v>
+      </c>
       <c r="AG65">
         <v>20</v>
       </c>
@@ -7184,6 +7229,9 @@
       </c>
       <c r="AC66">
         <v>300</v>
+      </c>
+      <c r="AF66">
+        <v>122</v>
       </c>
       <c r="AG66">
         <v>25</v>
@@ -7280,6 +7328,9 @@
       <c r="AC67">
         <v>452</v>
       </c>
+      <c r="AF67">
+        <v>182</v>
+      </c>
       <c r="AG67">
         <v>20</v>
       </c>
@@ -7764,6 +7815,9 @@
       <c r="AC72">
         <v>232</v>
       </c>
+      <c r="AF72">
+        <v>111</v>
+      </c>
       <c r="AG72">
         <v>113</v>
       </c>
@@ -8055,6 +8109,9 @@
       <c r="AC75">
         <v>352</v>
       </c>
+      <c r="AF75">
+        <v>128</v>
+      </c>
       <c r="AG75">
         <v>125</v>
       </c>
@@ -8913,6 +8970,9 @@
       <c r="Z84">
         <v>30</v>
       </c>
+      <c r="AF84">
+        <v>115</v>
+      </c>
       <c r="AG84">
         <v>116</v>
       </c>
@@ -9005,6 +9065,9 @@
       <c r="Z85">
         <v>35</v>
       </c>
+      <c r="AF85">
+        <v>117</v>
+      </c>
       <c r="AG85">
         <v>111</v>
       </c>
@@ -9382,6 +9445,9 @@
       <c r="Z89">
         <v>5</v>
       </c>
+      <c r="AF89">
+        <v>98</v>
+      </c>
       <c r="AG89">
         <v>102</v>
       </c>
@@ -10044,6 +10110,9 @@
       <c r="Z96">
         <v>10</v>
       </c>
+      <c r="AF96">
+        <v>96</v>
+      </c>
       <c r="AG96">
         <v>108</v>
       </c>
@@ -11181,6 +11250,9 @@
       <c r="Z108">
         <v>3</v>
       </c>
+      <c r="AF108">
+        <v>89</v>
+      </c>
       <c r="AG108">
         <v>91</v>
       </c>
@@ -11273,6 +11345,9 @@
       <c r="Z109">
         <v>15</v>
       </c>
+      <c r="AF109">
+        <v>116</v>
+      </c>
       <c r="AG109">
         <v>141</v>
       </c>
@@ -11460,6 +11535,9 @@
       <c r="Z111">
         <v>5</v>
       </c>
+      <c r="AF111">
+        <v>95</v>
+      </c>
       <c r="AG111">
         <v>98</v>
       </c>
@@ -12297,6 +12375,9 @@
       <c r="Z120">
         <v>25</v>
       </c>
+      <c r="AF120">
+        <v>143</v>
+      </c>
       <c r="AG120">
         <v>126</v>
       </c>
@@ -12674,6 +12755,9 @@
       <c r="Z124">
         <v>5</v>
       </c>
+      <c r="AF124">
+        <v>93</v>
+      </c>
       <c r="AG124">
         <v>98</v>
       </c>
@@ -12861,6 +12945,9 @@
       <c r="Z126">
         <v>0</v>
       </c>
+      <c r="AF126">
+        <v>116</v>
+      </c>
       <c r="AG126">
         <v>111</v>
       </c>
@@ -13238,6 +13325,9 @@
       <c r="Z130">
         <v>15</v>
       </c>
+      <c r="AF130">
+        <v>115</v>
+      </c>
       <c r="AG130">
         <v>126</v>
       </c>
@@ -13330,6 +13420,9 @@
       <c r="Z131">
         <v>35</v>
       </c>
+      <c r="AF131">
+        <v>135</v>
+      </c>
       <c r="AG131">
         <v>124</v>
       </c>
@@ -13422,6 +13515,9 @@
       <c r="Z132">
         <v>35</v>
       </c>
+      <c r="AF132">
+        <v>105</v>
+      </c>
       <c r="AG132">
         <v>104</v>
       </c>
@@ -13609,6 +13705,9 @@
       <c r="Z134">
         <v>5</v>
       </c>
+      <c r="AF134">
+        <v>96</v>
+      </c>
       <c r="AG134">
         <v>101</v>
       </c>
@@ -14271,6 +14370,9 @@
       <c r="Z141">
         <v>35</v>
       </c>
+      <c r="AF141">
+        <v>132</v>
+      </c>
       <c r="AG141">
         <v>127</v>
       </c>
@@ -14648,6 +14750,9 @@
       <c r="Z145">
         <v>35</v>
       </c>
+      <c r="AF145">
+        <v>119</v>
+      </c>
       <c r="AG145">
         <v>146</v>
       </c>
@@ -14740,6 +14845,9 @@
       <c r="Z146">
         <v>35</v>
       </c>
+      <c r="AF146">
+        <v>145</v>
+      </c>
       <c r="AG146">
         <v>149</v>
       </c>
@@ -16067,6 +16175,9 @@
       <c r="Z160">
         <v>60</v>
       </c>
+      <c r="AF160">
+        <v>124</v>
+      </c>
       <c r="AG160">
         <v>143</v>
       </c>
@@ -16159,6 +16270,9 @@
       <c r="Z161">
         <v>60</v>
       </c>
+      <c r="AF161">
+        <v>145</v>
+      </c>
       <c r="AG161">
         <v>134</v>
       </c>
@@ -16251,6 +16365,9 @@
       <c r="Z162">
         <v>40</v>
       </c>
+      <c r="AF162">
+        <v>115</v>
+      </c>
       <c r="AG162">
         <v>137</v>
       </c>
@@ -16343,6 +16460,9 @@
       <c r="Z163">
         <v>30</v>
       </c>
+      <c r="AF163">
+        <v>150</v>
+      </c>
       <c r="AG163">
         <v>169</v>
       </c>
@@ -16435,6 +16555,9 @@
       <c r="Z164">
         <v>45</v>
       </c>
+      <c r="AF164">
+        <v>124</v>
+      </c>
       <c r="AG164">
         <v>136</v>
       </c>
@@ -16527,6 +16650,9 @@
       <c r="Z165" t="s">
         <v>35</v>
       </c>
+      <c r="AF165">
+        <v>119</v>
+      </c>
       <c r="AG165">
         <v>145</v>
       </c>
@@ -16619,6 +16745,9 @@
       <c r="Z166">
         <v>20</v>
       </c>
+      <c r="AF166">
+        <v>123</v>
+      </c>
       <c r="AG166">
         <v>137</v>
       </c>
@@ -16711,6 +16840,9 @@
       <c r="Z167">
         <v>30</v>
       </c>
+      <c r="AF167">
+        <v>129</v>
+      </c>
       <c r="AG167">
         <v>118</v>
       </c>
@@ -17088,6 +17220,9 @@
       <c r="Z171">
         <v>33</v>
       </c>
+      <c r="AF171">
+        <v>92</v>
+      </c>
       <c r="AG171">
         <v>100</v>
       </c>
@@ -17180,6 +17315,9 @@
       <c r="Z172">
         <v>15</v>
       </c>
+      <c r="AF172">
+        <v>115</v>
+      </c>
       <c r="AG172">
         <v>120</v>
       </c>
@@ -17367,6 +17505,9 @@
       <c r="Z174">
         <v>10</v>
       </c>
+      <c r="AF174">
+        <v>95</v>
+      </c>
       <c r="AG174">
         <v>109</v>
       </c>
@@ -17648,6 +17789,9 @@
       </c>
       <c r="Z177">
         <v>10</v>
+      </c>
+      <c r="AF177">
+        <v>105</v>
       </c>
       <c r="AG177">
         <v>103</v>

</xml_diff>

<commit_message>
Count missing data, create sig matrix, split fts
</commit_message>
<xml_diff>
--- a/CRIq_new_dataworksheet.xlsx
+++ b/CRIq_new_dataworksheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Thesis Work\CRIq_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\CRIq_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="10212"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -512,12 +512,12 @@
   <dimension ref="A1:AJ189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AJ450"/>
+      <selection sqref="A1:AJ189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -627,7 +627,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>181</v>
       </c>
@@ -734,7 +734,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>182</v>
       </c>
@@ -817,13 +817,13 @@
         <v>17</v>
       </c>
       <c r="AB3">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AC3">
         <v>236</v>
       </c>
       <c r="AF3">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AG3">
         <v>121</v>
@@ -838,7 +838,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>211</v>
       </c>
@@ -942,7 +942,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>212</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>307</v>
       </c>
       <c r="AF5">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AG5">
         <v>108</v>
@@ -1046,7 +1046,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>213</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>214</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>365</v>
       </c>
       <c r="AF7">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AG7">
         <v>124</v>
@@ -1254,7 +1254,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>215</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>216</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>217</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>218</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>241</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>272</v>
       </c>
       <c r="AF12">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AG12">
         <v>127</v>
@@ -1774,7 +1774,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>242</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>243</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>102</v>
       </c>
       <c r="AF14">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AG14">
         <v>122</v>
@@ -1982,7 +1982,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>244</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>288</v>
       </c>
       <c r="AF15">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AG15">
         <v>125</v>
@@ -2086,7 +2086,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>245</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>193</v>
       </c>
       <c r="AF16">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AG16">
         <v>132</v>
@@ -2190,7 +2190,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>246</v>
       </c>
@@ -2273,13 +2273,13 @@
         <v>26</v>
       </c>
       <c r="AB17">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC17">
         <v>288</v>
       </c>
       <c r="AF17">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AG17">
         <v>123</v>
@@ -2294,7 +2294,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>247</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>203</v>
       </c>
       <c r="AF18">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AG18">
         <v>108</v>
@@ -2398,7 +2398,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>248</v>
       </c>
@@ -2481,13 +2481,13 @@
         <v>26</v>
       </c>
       <c r="AB19">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AC19">
         <v>479</v>
       </c>
       <c r="AF19">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AG19">
         <v>143</v>
@@ -2502,7 +2502,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>249</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>250</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>277</v>
       </c>
       <c r="AF21">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="AG21">
         <v>135</v>
@@ -2710,7 +2710,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>251</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>26</v>
       </c>
       <c r="AB22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC22">
         <v>349</v>
@@ -2814,7 +2814,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>253</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>369</v>
       </c>
       <c r="AF23">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="AG23">
         <v>124</v>
@@ -2918,7 +2918,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>254</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>255</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>256</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>272</v>
       </c>
       <c r="AF26">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AG26">
         <v>101</v>
@@ -3230,7 +3230,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>257</v>
       </c>
@@ -3313,13 +3313,13 @@
         <v>21</v>
       </c>
       <c r="AB27">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC27">
         <v>253</v>
       </c>
       <c r="AF27">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="AG27">
         <v>125</v>
@@ -3334,7 +3334,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>258</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>61</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>62</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>63</v>
       </c>
@@ -3729,13 +3729,13 @@
         <v>35</v>
       </c>
       <c r="AB31">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="AC31">
         <v>307</v>
       </c>
       <c r="AF31">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="AG31">
         <v>165</v>
@@ -3750,7 +3750,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>64</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>487</v>
       </c>
       <c r="AF32">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AG32">
         <v>133</v>
@@ -3854,7 +3854,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>65</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>66</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>67</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>22</v>
       </c>
       <c r="AB35">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AC35">
         <v>210</v>
@@ -4166,7 +4166,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>68</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>69</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>70</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>71</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>72</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>91</v>
       </c>
@@ -4769,13 +4769,13 @@
         <v>22</v>
       </c>
       <c r="AB41">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AC41">
         <v>437</v>
       </c>
       <c r="AF41">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AG41">
         <v>130</v>
@@ -4790,7 +4790,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>92</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>93</v>
       </c>
@@ -4977,13 +4977,13 @@
         <v>16</v>
       </c>
       <c r="AB43">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AC43">
         <v>392</v>
       </c>
       <c r="AF43">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AG43">
         <v>116</v>
@@ -4998,7 +4998,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>94</v>
       </c>
@@ -5077,6 +5077,12 @@
       <c r="Z44">
         <v>5</v>
       </c>
+      <c r="AA44">
+        <v>20</v>
+      </c>
+      <c r="AB44">
+        <v>15</v>
+      </c>
       <c r="AC44">
         <v>45</v>
       </c>
@@ -5096,7 +5102,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>95</v>
       </c>
@@ -5175,11 +5181,17 @@
       <c r="Z45">
         <v>30</v>
       </c>
+      <c r="AA45">
+        <v>15</v>
+      </c>
+      <c r="AB45">
+        <v>15</v>
+      </c>
       <c r="AC45">
         <v>232</v>
       </c>
       <c r="AF45">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AG45">
         <v>105</v>
@@ -5194,7 +5206,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>96</v>
       </c>
@@ -5273,6 +5285,12 @@
       <c r="Z46">
         <v>5</v>
       </c>
+      <c r="AA46">
+        <v>20</v>
+      </c>
+      <c r="AB46">
+        <v>10</v>
+      </c>
       <c r="AC46">
         <v>40</v>
       </c>
@@ -5292,7 +5310,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>97</v>
       </c>
@@ -5371,6 +5389,12 @@
       <c r="Z47">
         <v>5</v>
       </c>
+      <c r="AA47">
+        <v>20</v>
+      </c>
+      <c r="AB47">
+        <v>10</v>
+      </c>
       <c r="AC47">
         <v>35</v>
       </c>
@@ -5390,7 +5414,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>98</v>
       </c>
@@ -5469,6 +5493,12 @@
       <c r="Z48">
         <v>5</v>
       </c>
+      <c r="AA48">
+        <v>20</v>
+      </c>
+      <c r="AB48">
+        <v>5</v>
+      </c>
       <c r="AC48">
         <v>35</v>
       </c>
@@ -5488,7 +5518,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>99</v>
       </c>
@@ -5567,11 +5597,17 @@
       <c r="Z49">
         <v>55</v>
       </c>
+      <c r="AA49">
+        <v>20</v>
+      </c>
+      <c r="AB49">
+        <v>50</v>
+      </c>
       <c r="AC49">
         <v>397</v>
       </c>
       <c r="AF49">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AG49">
         <v>133</v>
@@ -5586,7 +5622,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>421</v>
       </c>
@@ -5665,6 +5701,12 @@
       <c r="Z50">
         <v>10</v>
       </c>
+      <c r="AA50">
+        <v>20</v>
+      </c>
+      <c r="AB50">
+        <v>25</v>
+      </c>
       <c r="AC50">
         <v>75</v>
       </c>
@@ -5684,7 +5726,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>422</v>
       </c>
@@ -5763,11 +5805,17 @@
       <c r="Z51">
         <v>45</v>
       </c>
+      <c r="AA51">
+        <v>25</v>
+      </c>
+      <c r="AB51">
+        <v>35</v>
+      </c>
       <c r="AC51">
         <v>392</v>
       </c>
       <c r="AF51">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AG51">
         <v>136</v>
@@ -5782,7 +5830,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>423</v>
       </c>
@@ -5861,11 +5909,17 @@
       <c r="Z52">
         <v>45</v>
       </c>
+      <c r="AA52">
+        <v>15</v>
+      </c>
+      <c r="AB52">
+        <v>40</v>
+      </c>
       <c r="AC52">
         <v>392</v>
       </c>
       <c r="AF52">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AG52">
         <v>112</v>
@@ -5880,7 +5934,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>424</v>
       </c>
@@ -5959,6 +6013,12 @@
       <c r="Z53">
         <v>5</v>
       </c>
+      <c r="AA53">
+        <v>21</v>
+      </c>
+      <c r="AB53">
+        <v>0</v>
+      </c>
       <c r="AC53">
         <v>75</v>
       </c>
@@ -5978,7 +6038,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>425</v>
       </c>
@@ -6057,11 +6117,17 @@
       <c r="Z54">
         <v>55</v>
       </c>
+      <c r="AA54">
+        <v>15</v>
+      </c>
+      <c r="AB54">
+        <v>55</v>
+      </c>
       <c r="AC54">
         <v>523</v>
       </c>
       <c r="AF54">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AG54">
         <v>123</v>
@@ -6076,7 +6142,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>426</v>
       </c>
@@ -6155,11 +6221,17 @@
       <c r="Z55">
         <v>45</v>
       </c>
+      <c r="AA55">
+        <v>20</v>
+      </c>
+      <c r="AB55">
+        <v>45</v>
+      </c>
       <c r="AC55">
         <v>383</v>
       </c>
       <c r="AF55">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AG55">
         <v>116</v>
@@ -6174,7 +6246,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>427</v>
       </c>
@@ -6253,6 +6325,12 @@
       <c r="Z56">
         <v>15</v>
       </c>
+      <c r="AA56">
+        <v>26</v>
+      </c>
+      <c r="AB56">
+        <v>5</v>
+      </c>
       <c r="AC56">
         <v>110</v>
       </c>
@@ -6272,7 +6350,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1</v>
       </c>
@@ -6351,11 +6429,17 @@
       <c r="Z57">
         <v>30</v>
       </c>
+      <c r="AA57">
+        <v>24</v>
+      </c>
+      <c r="AB57">
+        <v>40</v>
+      </c>
       <c r="AC57">
         <v>277</v>
       </c>
       <c r="AF57">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AG57">
         <v>130</v>
@@ -6370,7 +6454,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2</v>
       </c>
@@ -6449,6 +6533,12 @@
       <c r="Z58">
         <v>35</v>
       </c>
+      <c r="AA58">
+        <v>2</v>
+      </c>
+      <c r="AB58">
+        <v>35</v>
+      </c>
       <c r="AC58">
         <v>316</v>
       </c>
@@ -6468,7 +6558,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>3</v>
       </c>
@@ -6547,6 +6637,12 @@
       <c r="Z59">
         <v>10</v>
       </c>
+      <c r="AA59">
+        <v>20</v>
+      </c>
+      <c r="AB59">
+        <v>10</v>
+      </c>
       <c r="AC59">
         <v>80</v>
       </c>
@@ -6566,7 +6662,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>5</v>
       </c>
@@ -6645,6 +6741,12 @@
       <c r="Z60">
         <v>10</v>
       </c>
+      <c r="AA60">
+        <v>26</v>
+      </c>
+      <c r="AB60">
+        <v>10</v>
+      </c>
       <c r="AC60">
         <v>105</v>
       </c>
@@ -6664,7 +6766,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>6</v>
       </c>
@@ -6743,11 +6845,17 @@
       <c r="Z61">
         <v>45</v>
       </c>
+      <c r="AA61">
+        <v>20</v>
+      </c>
+      <c r="AB61">
+        <v>35</v>
+      </c>
       <c r="AC61">
         <v>407</v>
       </c>
       <c r="AF61">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AG61">
         <v>132</v>
@@ -6762,7 +6870,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>31</v>
       </c>
@@ -6841,6 +6949,12 @@
       <c r="Z62">
         <v>45</v>
       </c>
+      <c r="AA62">
+        <v>20</v>
+      </c>
+      <c r="AB62">
+        <v>50</v>
+      </c>
       <c r="AC62">
         <v>237</v>
       </c>
@@ -6857,7 +6971,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>32</v>
       </c>
@@ -6936,6 +7050,12 @@
       <c r="Z63">
         <v>50</v>
       </c>
+      <c r="AA63">
+        <v>20</v>
+      </c>
+      <c r="AB63">
+        <v>50</v>
+      </c>
       <c r="AC63">
         <v>489</v>
       </c>
@@ -6952,7 +7072,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>33</v>
       </c>
@@ -7031,6 +7151,12 @@
       <c r="Z64">
         <v>50</v>
       </c>
+      <c r="AA64">
+        <v>20</v>
+      </c>
+      <c r="AB64">
+        <v>40</v>
+      </c>
       <c r="AC64">
         <v>330</v>
       </c>
@@ -7050,7 +7176,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>34</v>
       </c>
@@ -7129,6 +7255,12 @@
       <c r="Z65">
         <v>45</v>
       </c>
+      <c r="AA65">
+        <v>20</v>
+      </c>
+      <c r="AB65">
+        <v>30</v>
+      </c>
       <c r="AC65">
         <v>199</v>
       </c>
@@ -7148,7 +7280,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>35</v>
       </c>
@@ -7227,6 +7359,12 @@
       <c r="Z66">
         <v>40</v>
       </c>
+      <c r="AA66">
+        <v>20</v>
+      </c>
+      <c r="AB66">
+        <v>25</v>
+      </c>
       <c r="AC66">
         <v>300</v>
       </c>
@@ -7246,7 +7384,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>36</v>
       </c>
@@ -7325,6 +7463,12 @@
       <c r="Z67">
         <v>35</v>
       </c>
+      <c r="AA67">
+        <v>20</v>
+      </c>
+      <c r="AB67">
+        <v>15</v>
+      </c>
       <c r="AC67">
         <v>452</v>
       </c>
@@ -7344,7 +7488,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>37</v>
       </c>
@@ -7423,6 +7567,12 @@
       <c r="Z68">
         <v>40</v>
       </c>
+      <c r="AA68">
+        <v>15</v>
+      </c>
+      <c r="AB68">
+        <v>30</v>
+      </c>
       <c r="AC68">
         <v>297</v>
       </c>
@@ -7439,7 +7589,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>73</v>
       </c>
@@ -7518,11 +7668,17 @@
       <c r="Z69">
         <v>60</v>
       </c>
+      <c r="AA69">
+        <v>18</v>
+      </c>
+      <c r="AB69">
+        <v>35</v>
+      </c>
       <c r="AC69">
         <v>432</v>
       </c>
       <c r="AF69">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AG69">
         <v>119</v>
@@ -7537,7 +7693,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>331</v>
       </c>
@@ -7616,11 +7772,17 @@
       <c r="Z70">
         <v>25</v>
       </c>
+      <c r="AA70">
+        <v>21</v>
+      </c>
+      <c r="AB70">
+        <v>40</v>
+      </c>
       <c r="AC70">
         <v>121</v>
       </c>
       <c r="AF70">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AG70">
         <v>111</v>
@@ -7635,7 +7797,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>302</v>
       </c>
@@ -7714,11 +7876,17 @@
       <c r="Z71">
         <v>30</v>
       </c>
+      <c r="AA71">
+        <v>23</v>
+      </c>
+      <c r="AB71">
+        <v>35</v>
+      </c>
       <c r="AC71">
         <v>257</v>
       </c>
       <c r="AF71">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AG71">
         <v>119</v>
@@ -7733,7 +7901,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>303</v>
       </c>
@@ -7812,11 +7980,17 @@
       <c r="Z72">
         <v>0</v>
       </c>
+      <c r="AA72">
+        <v>20</v>
+      </c>
+      <c r="AB72">
+        <v>45</v>
+      </c>
       <c r="AC72">
         <v>232</v>
       </c>
       <c r="AF72">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="AG72">
         <v>113</v>
@@ -7831,7 +8005,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>364</v>
       </c>
@@ -7910,11 +8084,17 @@
       <c r="Z73">
         <v>45</v>
       </c>
+      <c r="AA73">
+        <v>26</v>
+      </c>
+      <c r="AB73">
+        <v>110</v>
+      </c>
       <c r="AC73">
         <v>352</v>
       </c>
       <c r="AF73">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AG73">
         <v>141</v>
@@ -7929,7 +8109,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>365</v>
       </c>
@@ -8008,11 +8188,17 @@
       <c r="Z74">
         <v>45</v>
       </c>
+      <c r="AA74">
+        <v>30</v>
+      </c>
+      <c r="AB74">
+        <v>70</v>
+      </c>
       <c r="AC74">
         <v>382</v>
       </c>
       <c r="AF74">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="AG74">
         <v>151</v>
@@ -8027,7 +8213,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>366</v>
       </c>
@@ -8106,11 +8292,17 @@
       <c r="Z75">
         <v>45</v>
       </c>
+      <c r="AA75">
+        <v>20</v>
+      </c>
+      <c r="AB75">
+        <v>35</v>
+      </c>
       <c r="AC75">
         <v>352</v>
       </c>
       <c r="AF75">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AG75">
         <v>125</v>
@@ -8125,7 +8317,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>367</v>
       </c>
@@ -8204,11 +8396,17 @@
       <c r="Z76">
         <v>0</v>
       </c>
+      <c r="AA76">
+        <v>20</v>
+      </c>
+      <c r="AB76">
+        <v>65</v>
+      </c>
       <c r="AC76">
         <v>252</v>
       </c>
       <c r="AF76">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AG76">
         <v>115</v>
@@ -8223,7 +8421,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>368</v>
       </c>
@@ -8302,11 +8500,17 @@
       <c r="Z77">
         <v>55</v>
       </c>
+      <c r="AA77">
+        <v>27</v>
+      </c>
+      <c r="AB77">
+        <v>50</v>
+      </c>
       <c r="AC77">
         <v>432</v>
       </c>
       <c r="AF77">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AG77">
         <v>151</v>
@@ -8321,7 +8525,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>369</v>
       </c>
@@ -8400,8 +8604,17 @@
       <c r="Z78">
         <v>45</v>
       </c>
+      <c r="AA78">
+        <v>29</v>
+      </c>
+      <c r="AB78">
+        <v>45</v>
+      </c>
+      <c r="AC78">
+        <v>257</v>
+      </c>
       <c r="AF78">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AG78">
         <v>144</v>
@@ -8416,7 +8629,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>370</v>
       </c>
@@ -8495,6 +8708,15 @@
       <c r="Z79">
         <v>5</v>
       </c>
+      <c r="AA79">
+        <v>21</v>
+      </c>
+      <c r="AB79">
+        <v>15</v>
+      </c>
+      <c r="AC79">
+        <v>40</v>
+      </c>
       <c r="AF79">
         <v>101</v>
       </c>
@@ -8511,7 +8733,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>371</v>
       </c>
@@ -8590,8 +8812,17 @@
       <c r="Z80">
         <v>35</v>
       </c>
+      <c r="AA80">
+        <v>21</v>
+      </c>
+      <c r="AB80">
+        <v>35</v>
+      </c>
+      <c r="AC80">
+        <v>332</v>
+      </c>
       <c r="AF80">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AG80">
         <v>118</v>
@@ -8606,7 +8837,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>372</v>
       </c>
@@ -8685,6 +8916,15 @@
       <c r="Z81">
         <v>40</v>
       </c>
+      <c r="AA81">
+        <v>29</v>
+      </c>
+      <c r="AB81">
+        <v>50</v>
+      </c>
+      <c r="AC81">
+        <v>270</v>
+      </c>
       <c r="AF81">
         <v>139</v>
       </c>
@@ -8701,7 +8941,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>373</v>
       </c>
@@ -8780,6 +9020,15 @@
       <c r="Z82">
         <v>5</v>
       </c>
+      <c r="AA82">
+        <v>20</v>
+      </c>
+      <c r="AB82">
+        <v>10</v>
+      </c>
+      <c r="AC82">
+        <v>40</v>
+      </c>
       <c r="AF82">
         <v>99</v>
       </c>
@@ -8796,7 +9045,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>374</v>
       </c>
@@ -8875,6 +9124,15 @@
       <c r="Z83">
         <v>5</v>
       </c>
+      <c r="AA83">
+        <v>20</v>
+      </c>
+      <c r="AB83">
+        <v>5</v>
+      </c>
+      <c r="AC83">
+        <v>35</v>
+      </c>
       <c r="AF83">
         <v>97</v>
       </c>
@@ -8891,7 +9149,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>375</v>
       </c>
@@ -8970,8 +9228,17 @@
       <c r="Z84">
         <v>30</v>
       </c>
+      <c r="AA84">
+        <v>20</v>
+      </c>
+      <c r="AB84">
+        <v>25</v>
+      </c>
+      <c r="AC84">
+        <v>232</v>
+      </c>
       <c r="AF84">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AG84">
         <v>116</v>
@@ -8986,7 +9253,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>376</v>
       </c>
@@ -9065,8 +9332,17 @@
       <c r="Z85">
         <v>35</v>
       </c>
+      <c r="AA85">
+        <v>15</v>
+      </c>
+      <c r="AB85">
+        <v>35</v>
+      </c>
+      <c r="AC85">
+        <v>242</v>
+      </c>
       <c r="AF85">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="AG85">
         <v>111</v>
@@ -9081,7 +9357,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="86" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>377</v>
       </c>
@@ -9160,8 +9436,17 @@
       <c r="Z86">
         <v>35</v>
       </c>
+      <c r="AA86">
+        <v>20</v>
+      </c>
+      <c r="AB86">
+        <v>40</v>
+      </c>
+      <c r="AC86">
+        <v>248</v>
+      </c>
       <c r="AF86">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AG86">
         <v>114</v>
@@ -9176,7 +9461,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="87" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>378</v>
       </c>
@@ -9255,8 +9540,17 @@
       <c r="Z87">
         <v>40</v>
       </c>
+      <c r="AA87">
+        <v>25</v>
+      </c>
+      <c r="AB87">
+        <v>40</v>
+      </c>
+      <c r="AC87">
+        <v>278</v>
+      </c>
       <c r="AF87">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="AG87">
         <v>132</v>
@@ -9271,7 +9565,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="88" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>379</v>
       </c>
@@ -9350,8 +9644,17 @@
       <c r="Z88">
         <v>40</v>
       </c>
+      <c r="AA88">
+        <v>15</v>
+      </c>
+      <c r="AB88">
+        <v>45</v>
+      </c>
+      <c r="AC88">
+        <v>363</v>
+      </c>
       <c r="AF88">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AG88">
         <v>109</v>
@@ -9366,7 +9669,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>271</v>
       </c>
@@ -9445,6 +9748,15 @@
       <c r="Z89">
         <v>5</v>
       </c>
+      <c r="AA89">
+        <v>20</v>
+      </c>
+      <c r="AB89">
+        <v>10</v>
+      </c>
+      <c r="AC89">
+        <v>35</v>
+      </c>
       <c r="AF89">
         <v>98</v>
       </c>
@@ -9461,7 +9773,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>272</v>
       </c>
@@ -9540,6 +9852,15 @@
       <c r="Z90">
         <v>5</v>
       </c>
+      <c r="AA90">
+        <v>20</v>
+      </c>
+      <c r="AB90">
+        <v>15</v>
+      </c>
+      <c r="AC90">
+        <v>25</v>
+      </c>
       <c r="AF90">
         <v>98</v>
       </c>
@@ -9556,7 +9877,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="91" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>273</v>
       </c>
@@ -9635,6 +9956,15 @@
       <c r="Z91">
         <v>0</v>
       </c>
+      <c r="AA91">
+        <v>15</v>
+      </c>
+      <c r="AB91">
+        <v>10</v>
+      </c>
+      <c r="AC91">
+        <v>55</v>
+      </c>
       <c r="AF91">
         <v>90</v>
       </c>
@@ -9651,7 +9981,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>274</v>
       </c>
@@ -9730,6 +10060,15 @@
       <c r="Z92">
         <v>5</v>
       </c>
+      <c r="AA92">
+        <v>15</v>
+      </c>
+      <c r="AB92">
+        <v>5</v>
+      </c>
+      <c r="AC92">
+        <v>80</v>
+      </c>
       <c r="AF92">
         <v>92</v>
       </c>
@@ -9746,7 +10085,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>275</v>
       </c>
@@ -9825,8 +10164,17 @@
       <c r="Z93">
         <v>45</v>
       </c>
+      <c r="AA93">
+        <v>30</v>
+      </c>
+      <c r="AB93">
+        <v>50</v>
+      </c>
+      <c r="AC93">
+        <v>367</v>
+      </c>
       <c r="AF93">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="AG93">
         <v>158</v>
@@ -9841,7 +10189,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="94" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>276</v>
       </c>
@@ -9920,8 +10268,17 @@
       <c r="Z94">
         <v>50</v>
       </c>
+      <c r="AA94">
+        <v>20</v>
+      </c>
+      <c r="AB94">
+        <v>60</v>
+      </c>
+      <c r="AC94">
+        <v>289</v>
+      </c>
       <c r="AF94">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AG94">
         <v>125</v>
@@ -9936,7 +10293,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="95" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>277</v>
       </c>
@@ -10015,6 +10372,15 @@
       <c r="Z95">
         <v>15</v>
       </c>
+      <c r="AA95">
+        <v>20</v>
+      </c>
+      <c r="AB95">
+        <v>15</v>
+      </c>
+      <c r="AC95">
+        <v>80</v>
+      </c>
       <c r="AF95">
         <v>106</v>
       </c>
@@ -10031,7 +10397,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>278</v>
       </c>
@@ -10110,6 +10476,15 @@
       <c r="Z96">
         <v>10</v>
       </c>
+      <c r="AA96">
+        <v>20</v>
+      </c>
+      <c r="AB96">
+        <v>5</v>
+      </c>
+      <c r="AC96">
+        <v>35</v>
+      </c>
       <c r="AF96">
         <v>96</v>
       </c>
@@ -10126,7 +10501,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>279</v>
       </c>
@@ -10205,8 +10580,17 @@
       <c r="Z97">
         <v>50</v>
       </c>
+      <c r="AA97">
+        <v>35</v>
+      </c>
+      <c r="AB97">
+        <v>40</v>
+      </c>
+      <c r="AC97">
+        <v>257</v>
+      </c>
       <c r="AF97">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AG97">
         <v>155</v>
@@ -10221,7 +10605,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="98" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>301</v>
       </c>
@@ -10300,6 +10684,15 @@
       <c r="Z98">
         <v>20</v>
       </c>
+      <c r="AA98">
+        <v>20</v>
+      </c>
+      <c r="AB98">
+        <v>25</v>
+      </c>
+      <c r="AC98">
+        <v>130</v>
+      </c>
       <c r="AF98">
         <v>104</v>
       </c>
@@ -10316,7 +10709,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>302</v>
       </c>
@@ -10395,6 +10788,15 @@
       <c r="Z99">
         <v>10</v>
       </c>
+      <c r="AA99">
+        <v>20</v>
+      </c>
+      <c r="AB99">
+        <v>5</v>
+      </c>
+      <c r="AC99">
+        <v>60</v>
+      </c>
       <c r="AF99">
         <v>99</v>
       </c>
@@ -10411,7 +10813,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="100" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>303</v>
       </c>
@@ -10490,6 +10892,15 @@
       <c r="Z100">
         <v>5</v>
       </c>
+      <c r="AA100">
+        <v>15</v>
+      </c>
+      <c r="AB100">
+        <v>5</v>
+      </c>
+      <c r="AC100">
+        <v>25</v>
+      </c>
       <c r="AF100">
         <v>90</v>
       </c>
@@ -10506,7 +10917,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>304</v>
       </c>
@@ -10585,6 +10996,15 @@
       <c r="Z101">
         <v>5</v>
       </c>
+      <c r="AA101">
+        <v>15</v>
+      </c>
+      <c r="AB101">
+        <v>5</v>
+      </c>
+      <c r="AC101">
+        <v>25</v>
+      </c>
       <c r="AF101">
         <v>90</v>
       </c>
@@ -10601,7 +11021,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>305</v>
       </c>
@@ -10680,6 +11100,15 @@
       <c r="Z102">
         <v>5</v>
       </c>
+      <c r="AA102">
+        <v>15</v>
+      </c>
+      <c r="AB102">
+        <v>5</v>
+      </c>
+      <c r="AC102">
+        <v>35</v>
+      </c>
       <c r="AF102">
         <v>89</v>
       </c>
@@ -10696,7 +11125,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>306</v>
       </c>
@@ -10775,8 +11204,17 @@
       <c r="Z103">
         <v>5</v>
       </c>
+      <c r="AA103">
+        <v>15</v>
+      </c>
+      <c r="AB103">
+        <v>35</v>
+      </c>
+      <c r="AC103">
+        <v>87</v>
+      </c>
       <c r="AF103">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AG103">
         <v>98</v>
@@ -10791,7 +11229,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="104" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>307</v>
       </c>
@@ -10870,6 +11308,15 @@
       <c r="Z104">
         <v>5</v>
       </c>
+      <c r="AA104">
+        <v>20</v>
+      </c>
+      <c r="AB104">
+        <v>10</v>
+      </c>
+      <c r="AC104">
+        <v>40</v>
+      </c>
       <c r="AF104">
         <v>99</v>
       </c>
@@ -10886,7 +11333,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="105" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>308</v>
       </c>
@@ -10965,6 +11412,15 @@
       <c r="Z105">
         <v>5</v>
       </c>
+      <c r="AA105">
+        <v>20</v>
+      </c>
+      <c r="AB105">
+        <v>5</v>
+      </c>
+      <c r="AC105">
+        <v>35</v>
+      </c>
       <c r="AF105">
         <v>97</v>
       </c>
@@ -10981,7 +11437,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="106" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>309</v>
       </c>
@@ -11060,6 +11516,15 @@
       <c r="Z106">
         <v>5</v>
       </c>
+      <c r="AA106">
+        <v>15</v>
+      </c>
+      <c r="AB106">
+        <v>5</v>
+      </c>
+      <c r="AC106">
+        <v>35</v>
+      </c>
       <c r="AF106">
         <v>91</v>
       </c>
@@ -11076,7 +11541,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="107" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>310</v>
       </c>
@@ -11155,8 +11620,17 @@
       <c r="Z107">
         <v>5</v>
       </c>
+      <c r="AA107">
+        <v>20</v>
+      </c>
+      <c r="AB107">
+        <v>5</v>
+      </c>
+      <c r="AC107">
+        <v>26</v>
+      </c>
       <c r="AF107">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="AG107">
         <v>101</v>
@@ -11171,7 +11645,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="108" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>332</v>
       </c>
@@ -11250,6 +11724,15 @@
       <c r="Z108">
         <v>3</v>
       </c>
+      <c r="AA108">
+        <v>15</v>
+      </c>
+      <c r="AB108">
+        <v>5</v>
+      </c>
+      <c r="AC108">
+        <v>33</v>
+      </c>
       <c r="AF108">
         <v>89</v>
       </c>
@@ -11266,7 +11749,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="109" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>333</v>
       </c>
@@ -11345,6 +11828,15 @@
       <c r="Z109">
         <v>15</v>
       </c>
+      <c r="AA109">
+        <v>30</v>
+      </c>
+      <c r="AB109">
+        <v>15</v>
+      </c>
+      <c r="AC109">
+        <v>105</v>
+      </c>
       <c r="AF109">
         <v>116</v>
       </c>
@@ -11361,7 +11853,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="110" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>334</v>
       </c>
@@ -11440,6 +11932,15 @@
       <c r="Z110">
         <v>15</v>
       </c>
+      <c r="AA110">
+        <v>30</v>
+      </c>
+      <c r="AB110">
+        <v>20</v>
+      </c>
+      <c r="AC110">
+        <v>150</v>
+      </c>
       <c r="AF110">
         <v>122</v>
       </c>
@@ -11456,7 +11957,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="111" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>335</v>
       </c>
@@ -11535,6 +12036,15 @@
       <c r="Z111">
         <v>5</v>
       </c>
+      <c r="AA111">
+        <v>20</v>
+      </c>
+      <c r="AB111">
+        <v>5</v>
+      </c>
+      <c r="AC111">
+        <v>55</v>
+      </c>
       <c r="AF111">
         <v>95</v>
       </c>
@@ -11551,7 +12061,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="112" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>336</v>
       </c>
@@ -11630,8 +12140,17 @@
       <c r="Z112">
         <v>50</v>
       </c>
+      <c r="AA112">
+        <v>20</v>
+      </c>
+      <c r="AB112">
+        <v>35</v>
+      </c>
+      <c r="AC112">
+        <v>247</v>
+      </c>
       <c r="AF112">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AG112">
         <v>126</v>
@@ -11646,7 +12165,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="113" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>337</v>
       </c>
@@ -11725,8 +12244,17 @@
       <c r="Z113">
         <v>20</v>
       </c>
+      <c r="AA113">
+        <v>40</v>
+      </c>
+      <c r="AB113">
+        <v>35</v>
+      </c>
+      <c r="AC113">
+        <v>463</v>
+      </c>
       <c r="AF113">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AG113">
         <v>171</v>
@@ -11741,7 +12269,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="114" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>338</v>
       </c>
@@ -11820,8 +12348,17 @@
       <c r="Z114">
         <v>15</v>
       </c>
+      <c r="AA114">
+        <v>27</v>
+      </c>
+      <c r="AB114">
+        <v>30</v>
+      </c>
+      <c r="AC114">
+        <v>307</v>
+      </c>
       <c r="AF114">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="AG114">
         <v>121</v>
@@ -11836,7 +12373,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="115" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>339</v>
       </c>
@@ -11915,8 +12452,17 @@
       <c r="Z115">
         <v>25</v>
       </c>
+      <c r="AA115">
+        <v>29</v>
+      </c>
+      <c r="AB115">
+        <v>40</v>
+      </c>
+      <c r="AC115">
+        <v>233</v>
+      </c>
     </row>
-    <row r="116" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>340</v>
       </c>
@@ -11995,6 +12541,15 @@
       <c r="Z116">
         <v>5</v>
       </c>
+      <c r="AA116">
+        <v>20</v>
+      </c>
+      <c r="AB116">
+        <v>5</v>
+      </c>
+      <c r="AC116">
+        <v>90</v>
+      </c>
       <c r="AF116">
         <v>101</v>
       </c>
@@ -12011,7 +12566,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="117" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>533</v>
       </c>
@@ -12090,6 +12645,15 @@
       <c r="Z117">
         <v>10</v>
       </c>
+      <c r="AA117">
+        <v>26</v>
+      </c>
+      <c r="AB117">
+        <v>0</v>
+      </c>
+      <c r="AC117">
+        <v>85</v>
+      </c>
       <c r="AF117">
         <v>113</v>
       </c>
@@ -12106,7 +12670,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="118" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>534</v>
       </c>
@@ -12185,8 +12749,17 @@
       <c r="Z118">
         <v>55</v>
       </c>
+      <c r="AA118">
+        <v>22</v>
+      </c>
+      <c r="AB118">
+        <v>30</v>
+      </c>
+      <c r="AC118">
+        <v>648</v>
+      </c>
       <c r="AF118">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AG118">
         <v>140</v>
@@ -12201,7 +12774,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="119" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>535</v>
       </c>
@@ -12280,6 +12853,15 @@
       <c r="Z119">
         <v>40</v>
       </c>
+      <c r="AA119">
+        <v>18</v>
+      </c>
+      <c r="AB119">
+        <v>40</v>
+      </c>
+      <c r="AC119">
+        <v>215</v>
+      </c>
       <c r="AF119">
         <v>122</v>
       </c>
@@ -12296,7 +12878,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="120" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>428</v>
       </c>
@@ -12375,6 +12957,15 @@
       <c r="Z120">
         <v>25</v>
       </c>
+      <c r="AA120">
+        <v>20</v>
+      </c>
+      <c r="AB120">
+        <v>45</v>
+      </c>
+      <c r="AC120">
+        <v>410</v>
+      </c>
       <c r="AF120">
         <v>143</v>
       </c>
@@ -12391,7 +12982,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="121" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>429</v>
       </c>
@@ -12470,6 +13061,15 @@
       <c r="Z121">
         <v>10</v>
       </c>
+      <c r="AA121">
+        <v>20</v>
+      </c>
+      <c r="AB121">
+        <v>10</v>
+      </c>
+      <c r="AC121">
+        <v>80</v>
+      </c>
       <c r="AF121">
         <v>100</v>
       </c>
@@ -12486,7 +13086,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="122" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>430</v>
       </c>
@@ -12565,6 +13165,15 @@
       <c r="Z122">
         <v>10</v>
       </c>
+      <c r="AA122">
+        <v>20</v>
+      </c>
+      <c r="AB122">
+        <v>5</v>
+      </c>
+      <c r="AC122">
+        <v>55</v>
+      </c>
       <c r="AF122">
         <v>98</v>
       </c>
@@ -12581,7 +13190,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="123" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>403</v>
       </c>
@@ -12660,6 +13269,15 @@
       <c r="Z123">
         <v>5</v>
       </c>
+      <c r="AA123">
+        <v>15</v>
+      </c>
+      <c r="AB123">
+        <v>5</v>
+      </c>
+      <c r="AC123">
+        <v>30</v>
+      </c>
       <c r="AF123">
         <v>90</v>
       </c>
@@ -12676,7 +13294,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="124" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>402</v>
       </c>
@@ -12755,6 +13373,15 @@
       <c r="Z124">
         <v>5</v>
       </c>
+      <c r="AA124">
+        <v>20</v>
+      </c>
+      <c r="AB124">
+        <v>5</v>
+      </c>
+      <c r="AC124">
+        <v>40</v>
+      </c>
       <c r="AF124">
         <v>93</v>
       </c>
@@ -12771,7 +13398,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="125" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>401</v>
       </c>
@@ -12850,8 +13477,17 @@
       <c r="Z125">
         <v>45</v>
       </c>
+      <c r="AA125">
+        <v>20</v>
+      </c>
+      <c r="AB125">
+        <v>40</v>
+      </c>
+      <c r="AC125">
+        <v>313</v>
+      </c>
       <c r="AF125">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AG125">
         <v>123</v>
@@ -12866,7 +13502,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="126" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>400</v>
       </c>
@@ -12945,8 +13581,17 @@
       <c r="Z126">
         <v>0</v>
       </c>
+      <c r="AA126">
+        <v>10</v>
+      </c>
+      <c r="AB126">
+        <v>40</v>
+      </c>
+      <c r="AC126">
+        <v>298</v>
+      </c>
       <c r="AF126">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AG126">
         <v>111</v>
@@ -12961,7 +13606,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>399</v>
       </c>
@@ -13040,8 +13685,17 @@
       <c r="Z127">
         <v>25</v>
       </c>
+      <c r="AA127">
+        <v>20</v>
+      </c>
+      <c r="AB127">
+        <v>25</v>
+      </c>
+      <c r="AC127">
+        <v>252</v>
+      </c>
       <c r="AF127">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AG127">
         <v>112</v>
@@ -13056,7 +13710,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>398</v>
       </c>
@@ -13135,8 +13789,17 @@
       <c r="Z128">
         <v>35</v>
       </c>
+      <c r="AA128">
+        <v>43</v>
+      </c>
+      <c r="AB128">
+        <v>55</v>
+      </c>
+      <c r="AC128">
+        <v>471</v>
+      </c>
       <c r="AF128">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AG128">
         <v>164</v>
@@ -13151,7 +13814,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="129" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>391</v>
       </c>
@@ -13230,8 +13893,17 @@
       <c r="Z129">
         <v>0</v>
       </c>
+      <c r="AA129">
+        <v>17</v>
+      </c>
+      <c r="AB129">
+        <v>40</v>
+      </c>
+      <c r="AC129">
+        <v>302</v>
+      </c>
       <c r="AF129">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AG129">
         <v>106</v>
@@ -13246,7 +13918,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="130" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>397</v>
       </c>
@@ -13325,6 +13997,15 @@
       <c r="Z130">
         <v>15</v>
       </c>
+      <c r="AA130">
+        <v>25</v>
+      </c>
+      <c r="AB130">
+        <v>25</v>
+      </c>
+      <c r="AC130">
+        <v>125</v>
+      </c>
       <c r="AF130">
         <v>115</v>
       </c>
@@ -13341,7 +14022,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="131" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>396</v>
       </c>
@@ -13420,8 +14101,17 @@
       <c r="Z131">
         <v>35</v>
       </c>
+      <c r="AA131">
+        <v>20</v>
+      </c>
+      <c r="AB131">
+        <v>40</v>
+      </c>
+      <c r="AC131">
+        <v>400</v>
+      </c>
       <c r="AF131">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AG131">
         <v>124</v>
@@ -13436,7 +14126,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="132" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>395</v>
       </c>
@@ -13515,8 +14205,17 @@
       <c r="Z132">
         <v>35</v>
       </c>
+      <c r="AA132">
+        <v>12</v>
+      </c>
+      <c r="AB132">
+        <v>40</v>
+      </c>
+      <c r="AC132">
+        <v>223</v>
+      </c>
       <c r="AF132">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AG132">
         <v>104</v>
@@ -13531,7 +14230,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="133" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>394</v>
       </c>
@@ -13610,8 +14309,17 @@
       <c r="Z133">
         <v>25</v>
       </c>
+      <c r="AA133">
+        <v>18</v>
+      </c>
+      <c r="AB133">
+        <v>30</v>
+      </c>
+      <c r="AC133">
+        <v>202</v>
+      </c>
       <c r="AF133">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="AG133">
         <v>123</v>
@@ -13626,7 +14334,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="134" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>393</v>
       </c>
@@ -13705,6 +14413,15 @@
       <c r="Z134">
         <v>5</v>
       </c>
+      <c r="AA134">
+        <v>20</v>
+      </c>
+      <c r="AB134">
+        <v>10</v>
+      </c>
+      <c r="AC134">
+        <v>40</v>
+      </c>
       <c r="AF134">
         <v>96</v>
       </c>
@@ -13721,7 +14438,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="135" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>392</v>
       </c>
@@ -13800,8 +14517,17 @@
       <c r="Z135">
         <v>35</v>
       </c>
+      <c r="AA135">
+        <v>22</v>
+      </c>
+      <c r="AB135">
+        <v>35</v>
+      </c>
+      <c r="AC135">
+        <v>287</v>
+      </c>
       <c r="AF135">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AG135">
         <v>125</v>
@@ -13816,7 +14542,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="136" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>526</v>
       </c>
@@ -13895,6 +14621,15 @@
       <c r="Z136">
         <v>30</v>
       </c>
+      <c r="AA136">
+        <v>23</v>
+      </c>
+      <c r="AB136">
+        <v>30</v>
+      </c>
+      <c r="AC136">
+        <v>251</v>
+      </c>
       <c r="AF136">
         <v>130</v>
       </c>
@@ -13911,7 +14646,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="137" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>539</v>
       </c>
@@ -13990,6 +14725,15 @@
       <c r="Z137">
         <v>5</v>
       </c>
+      <c r="AA137">
+        <v>20</v>
+      </c>
+      <c r="AB137">
+        <v>5</v>
+      </c>
+      <c r="AC137">
+        <v>40</v>
+      </c>
       <c r="AF137">
         <v>96</v>
       </c>
@@ -14006,7 +14750,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="138" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>540</v>
       </c>
@@ -14085,6 +14829,15 @@
       <c r="Z138">
         <v>0</v>
       </c>
+      <c r="AA138">
+        <v>15</v>
+      </c>
+      <c r="AB138">
+        <v>5</v>
+      </c>
+      <c r="AC138">
+        <v>40</v>
+      </c>
       <c r="AF138">
         <v>91</v>
       </c>
@@ -14101,7 +14854,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="139" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>542</v>
       </c>
@@ -14180,8 +14933,17 @@
       <c r="Z139">
         <v>35</v>
       </c>
+      <c r="AA139">
+        <v>22</v>
+      </c>
+      <c r="AB139">
+        <v>45</v>
+      </c>
+      <c r="AC139">
+        <v>353</v>
+      </c>
       <c r="AF139">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AG139">
         <v>128</v>
@@ -14196,7 +14958,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="140" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>545</v>
       </c>
@@ -14275,8 +15037,17 @@
       <c r="Z140">
         <v>45</v>
       </c>
+      <c r="AA140">
+        <v>20</v>
+      </c>
+      <c r="AB140">
+        <v>50</v>
+      </c>
+      <c r="AC140">
+        <v>408</v>
+      </c>
       <c r="AF140">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AG140">
         <v>122</v>
@@ -14291,7 +15062,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>548</v>
       </c>
@@ -14370,8 +15141,17 @@
       <c r="Z141">
         <v>35</v>
       </c>
+      <c r="AA141">
+        <v>25</v>
+      </c>
+      <c r="AB141">
+        <v>30</v>
+      </c>
+      <c r="AC141">
+        <v>377</v>
+      </c>
       <c r="AF141">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AG141">
         <v>127</v>
@@ -14386,7 +15166,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="142" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>560</v>
       </c>
@@ -14465,8 +15245,17 @@
       <c r="Z142">
         <v>40</v>
       </c>
+      <c r="AA142">
+        <v>20</v>
+      </c>
+      <c r="AB142">
+        <v>35</v>
+      </c>
+      <c r="AC142">
+        <v>384</v>
+      </c>
       <c r="AF142">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AG142">
         <v>114</v>
@@ -14481,7 +15270,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="143" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>570</v>
       </c>
@@ -14560,8 +15349,17 @@
       <c r="Z143">
         <v>35</v>
       </c>
+      <c r="AA143">
+        <v>25</v>
+      </c>
+      <c r="AB143">
+        <v>35</v>
+      </c>
+      <c r="AC143">
+        <v>188</v>
+      </c>
       <c r="AF143">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AG143">
         <v>128</v>
@@ -14576,7 +15374,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="144" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>571</v>
       </c>
@@ -14655,8 +15453,17 @@
       <c r="Z144">
         <v>20</v>
       </c>
+      <c r="AA144">
+        <v>15</v>
+      </c>
+      <c r="AB144">
+        <v>15</v>
+      </c>
+      <c r="AC144">
+        <v>142</v>
+      </c>
       <c r="AF144">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AG144">
         <v>96</v>
@@ -14671,7 +15478,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="145" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>573</v>
       </c>
@@ -14750,6 +15557,15 @@
       <c r="Z145">
         <v>35</v>
       </c>
+      <c r="AA145">
+        <v>30</v>
+      </c>
+      <c r="AB145">
+        <v>35</v>
+      </c>
+      <c r="AC145">
+        <v>178</v>
+      </c>
       <c r="AF145">
         <v>119</v>
       </c>
@@ -14766,7 +15582,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="146" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>575</v>
       </c>
@@ -14845,6 +15661,15 @@
       <c r="Z146">
         <v>35</v>
       </c>
+      <c r="AA146">
+        <v>31</v>
+      </c>
+      <c r="AB146">
+        <v>5</v>
+      </c>
+      <c r="AC146">
+        <v>416</v>
+      </c>
       <c r="AF146">
         <v>145</v>
       </c>
@@ -14861,7 +15686,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>451</v>
       </c>
@@ -14940,6 +15765,15 @@
       <c r="Z147">
         <v>20</v>
       </c>
+      <c r="AA147">
+        <v>25</v>
+      </c>
+      <c r="AB147">
+        <v>20</v>
+      </c>
+      <c r="AC147">
+        <v>95</v>
+      </c>
       <c r="AF147">
         <v>108</v>
       </c>
@@ -14956,7 +15790,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="148" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>452</v>
       </c>
@@ -15035,8 +15869,17 @@
       <c r="Z148">
         <v>45</v>
       </c>
+      <c r="AA148">
+        <v>31</v>
+      </c>
+      <c r="AB148">
+        <v>35</v>
+      </c>
+      <c r="AC148">
+        <v>272</v>
+      </c>
       <c r="AF148">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AG148">
         <v>149</v>
@@ -15051,7 +15894,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="149" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>453</v>
       </c>
@@ -15130,6 +15973,15 @@
       <c r="Z149">
         <v>55</v>
       </c>
+      <c r="AA149">
+        <v>30</v>
+      </c>
+      <c r="AB149">
+        <v>50</v>
+      </c>
+      <c r="AC149">
+        <v>610</v>
+      </c>
       <c r="AF149">
         <v>164</v>
       </c>
@@ -15146,7 +15998,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="150" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>454</v>
       </c>
@@ -15225,6 +16077,15 @@
       <c r="Z150">
         <v>15</v>
       </c>
+      <c r="AA150">
+        <v>25</v>
+      </c>
+      <c r="AB150">
+        <v>20</v>
+      </c>
+      <c r="AC150">
+        <v>135</v>
+      </c>
       <c r="AF150">
         <v>111</v>
       </c>
@@ -15241,7 +16102,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="151" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>455</v>
       </c>
@@ -15320,8 +16181,17 @@
       <c r="Z151">
         <v>40</v>
       </c>
+      <c r="AA151">
+        <v>21</v>
+      </c>
+      <c r="AB151">
+        <v>50</v>
+      </c>
+      <c r="AC151">
+        <v>401</v>
+      </c>
       <c r="AF151">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AG151">
         <v>122</v>
@@ -15336,7 +16206,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="152" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>456</v>
       </c>
@@ -15415,8 +16285,17 @@
       <c r="Z152">
         <v>60</v>
       </c>
+      <c r="AA152">
+        <v>13</v>
+      </c>
+      <c r="AB152">
+        <v>55</v>
+      </c>
+      <c r="AC152">
+        <v>359</v>
+      </c>
       <c r="AF152">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AG152">
         <v>107</v>
@@ -15431,7 +16310,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="153" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>457</v>
       </c>
@@ -15510,8 +16389,17 @@
       <c r="Z153">
         <v>30</v>
       </c>
+      <c r="AA153">
+        <v>20</v>
+      </c>
+      <c r="AB153">
+        <v>25</v>
+      </c>
+      <c r="AC153">
+        <v>313</v>
+      </c>
       <c r="AF153">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AG153">
         <v>119</v>
@@ -15526,7 +16414,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="154" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>458</v>
       </c>
@@ -15605,8 +16493,17 @@
       <c r="Z154">
         <v>40</v>
       </c>
+      <c r="AA154">
+        <v>25</v>
+      </c>
+      <c r="AB154">
+        <v>35</v>
+      </c>
+      <c r="AC154">
+        <v>317</v>
+      </c>
       <c r="AF154">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AG154">
         <v>138</v>
@@ -15621,7 +16518,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="155" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>459</v>
       </c>
@@ -15700,6 +16597,15 @@
       <c r="Z155">
         <v>45</v>
       </c>
+      <c r="AA155">
+        <v>25</v>
+      </c>
+      <c r="AB155">
+        <v>75</v>
+      </c>
+      <c r="AC155">
+        <v>365</v>
+      </c>
       <c r="AF155">
         <v>155</v>
       </c>
@@ -15716,7 +16622,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="156" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>460</v>
       </c>
@@ -15795,6 +16701,15 @@
       <c r="Z156">
         <v>10</v>
       </c>
+      <c r="AA156">
+        <v>20</v>
+      </c>
+      <c r="AB156">
+        <v>15</v>
+      </c>
+      <c r="AC156">
+        <v>65</v>
+      </c>
       <c r="AF156">
         <v>100</v>
       </c>
@@ -15811,7 +16726,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="157" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>461</v>
       </c>
@@ -15890,8 +16805,17 @@
       <c r="Z157">
         <v>40</v>
       </c>
+      <c r="AA157">
+        <v>25</v>
+      </c>
+      <c r="AB157">
+        <v>40</v>
+      </c>
+      <c r="AC157">
+        <v>312</v>
+      </c>
       <c r="AF157">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AG157">
         <v>130</v>
@@ -15906,7 +16830,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="158" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>462</v>
       </c>
@@ -15985,8 +16909,17 @@
       <c r="Z158">
         <v>45</v>
       </c>
+      <c r="AA158">
+        <v>26</v>
+      </c>
+      <c r="AB158">
+        <v>40</v>
+      </c>
+      <c r="AC158">
+        <v>367</v>
+      </c>
       <c r="AF158">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AG158">
         <v>133</v>
@@ -16001,7 +16934,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="159" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>481</v>
       </c>
@@ -16080,6 +17013,15 @@
       <c r="Z159">
         <v>20</v>
       </c>
+      <c r="AA159">
+        <v>31</v>
+      </c>
+      <c r="AB159">
+        <v>35</v>
+      </c>
+      <c r="AC159">
+        <v>225</v>
+      </c>
       <c r="AF159">
         <v>141</v>
       </c>
@@ -16096,7 +17038,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="160" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>121</v>
       </c>
@@ -16175,8 +17117,17 @@
       <c r="Z160">
         <v>60</v>
       </c>
+      <c r="AA160">
+        <v>0</v>
+      </c>
+      <c r="AB160">
+        <v>0</v>
+      </c>
+      <c r="AC160">
+        <v>357</v>
+      </c>
       <c r="AF160">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AG160">
         <v>143</v>
@@ -16191,7 +17142,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="161" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>122</v>
       </c>
@@ -16270,8 +17221,17 @@
       <c r="Z161">
         <v>60</v>
       </c>
+      <c r="AA161">
+        <v>0</v>
+      </c>
+      <c r="AB161">
+        <v>35</v>
+      </c>
+      <c r="AC161">
+        <v>556</v>
+      </c>
       <c r="AF161">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AG161">
         <v>134</v>
@@ -16286,7 +17246,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="162" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>123</v>
       </c>
@@ -16365,8 +17325,17 @@
       <c r="Z162">
         <v>40</v>
       </c>
+      <c r="AA162">
+        <v>0</v>
+      </c>
+      <c r="AB162">
+        <v>0</v>
+      </c>
+      <c r="AC162">
+        <v>252</v>
+      </c>
       <c r="AF162">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AG162">
         <v>137</v>
@@ -16381,7 +17350,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="163" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>124</v>
       </c>
@@ -16460,6 +17429,15 @@
       <c r="Z163">
         <v>30</v>
       </c>
+      <c r="AA163">
+        <v>0</v>
+      </c>
+      <c r="AB163">
+        <v>25</v>
+      </c>
+      <c r="AC163">
+        <v>390</v>
+      </c>
       <c r="AF163">
         <v>150</v>
       </c>
@@ -16476,7 +17454,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="164" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>125</v>
       </c>
@@ -16555,8 +17533,17 @@
       <c r="Z164">
         <v>45</v>
       </c>
+      <c r="AA164">
+        <v>0</v>
+      </c>
+      <c r="AB164">
+        <v>20</v>
+      </c>
+      <c r="AC164">
+        <v>343</v>
+      </c>
       <c r="AF164">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AG164">
         <v>136</v>
@@ -16571,7 +17558,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="165" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>151</v>
       </c>
@@ -16650,6 +17637,15 @@
       <c r="Z165" t="s">
         <v>35</v>
       </c>
+      <c r="AA165">
+        <v>20</v>
+      </c>
+      <c r="AB165">
+        <v>45</v>
+      </c>
+      <c r="AC165">
+        <v>288</v>
+      </c>
       <c r="AF165">
         <v>119</v>
       </c>
@@ -16666,7 +17662,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="166" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>152</v>
       </c>
@@ -16745,6 +17741,15 @@
       <c r="Z166">
         <v>20</v>
       </c>
+      <c r="AA166">
+        <v>27</v>
+      </c>
+      <c r="AB166">
+        <v>0</v>
+      </c>
+      <c r="AC166">
+        <v>246</v>
+      </c>
       <c r="AF166">
         <v>123</v>
       </c>
@@ -16761,7 +17766,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="167" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>153</v>
       </c>
@@ -16840,6 +17845,15 @@
       <c r="Z167">
         <v>30</v>
       </c>
+      <c r="AA167">
+        <v>20</v>
+      </c>
+      <c r="AB167">
+        <v>0</v>
+      </c>
+      <c r="AC167">
+        <v>240</v>
+      </c>
       <c r="AF167">
         <v>129</v>
       </c>
@@ -16856,7 +17870,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="168" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>100</v>
       </c>
@@ -16935,6 +17949,15 @@
       <c r="Z168">
         <v>5</v>
       </c>
+      <c r="AA168">
+        <v>20</v>
+      </c>
+      <c r="AB168">
+        <v>10</v>
+      </c>
+      <c r="AC168">
+        <v>45</v>
+      </c>
       <c r="AF168">
         <v>99</v>
       </c>
@@ -16951,7 +17974,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="169" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>101</v>
       </c>
@@ -17030,6 +18053,15 @@
       <c r="Z169">
         <v>55</v>
       </c>
+      <c r="AA169">
+        <v>25</v>
+      </c>
+      <c r="AB169">
+        <v>50</v>
+      </c>
+      <c r="AC169">
+        <v>455</v>
+      </c>
       <c r="AF169">
         <v>142</v>
       </c>
@@ -17046,7 +18078,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="170" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>426</v>
       </c>
@@ -17125,8 +18157,17 @@
       <c r="Z170">
         <v>45</v>
       </c>
+      <c r="AA170">
+        <v>20</v>
+      </c>
+      <c r="AB170">
+        <v>50</v>
+      </c>
+      <c r="AC170">
+        <v>383</v>
+      </c>
       <c r="AF170">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AG170">
         <v>116</v>
@@ -17141,7 +18182,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="171" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>500</v>
       </c>
@@ -17220,6 +18261,15 @@
       <c r="Z171">
         <v>33</v>
       </c>
+      <c r="AA171">
+        <v>0</v>
+      </c>
+      <c r="AB171">
+        <v>5</v>
+      </c>
+      <c r="AC171">
+        <v>253</v>
+      </c>
       <c r="AF171">
         <v>92</v>
       </c>
@@ -17236,7 +18286,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="172" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>520</v>
       </c>
@@ -17315,6 +18365,15 @@
       <c r="Z172">
         <v>15</v>
       </c>
+      <c r="AA172">
+        <v>25.5</v>
+      </c>
+      <c r="AB172">
+        <v>25</v>
+      </c>
+      <c r="AC172">
+        <v>120</v>
+      </c>
       <c r="AF172">
         <v>115</v>
       </c>
@@ -17331,7 +18390,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="173" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>521</v>
       </c>
@@ -17410,6 +18469,15 @@
       <c r="Z173">
         <v>10</v>
       </c>
+      <c r="AA173">
+        <v>25</v>
+      </c>
+      <c r="AB173">
+        <v>10</v>
+      </c>
+      <c r="AC173">
+        <v>105</v>
+      </c>
       <c r="AF173">
         <v>108</v>
       </c>
@@ -17426,7 +18494,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="174" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>525</v>
       </c>
@@ -17505,6 +18573,15 @@
       <c r="Z174">
         <v>10</v>
       </c>
+      <c r="AA174">
+        <v>20</v>
+      </c>
+      <c r="AB174">
+        <v>5</v>
+      </c>
+      <c r="AC174">
+        <v>30</v>
+      </c>
       <c r="AF174">
         <v>95</v>
       </c>
@@ -17521,7 +18598,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="175" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>527</v>
       </c>
@@ -17600,8 +18677,17 @@
       <c r="Z175">
         <v>45</v>
       </c>
+      <c r="AA175">
+        <v>20</v>
+      </c>
+      <c r="AB175">
+        <v>35</v>
+      </c>
+      <c r="AC175">
+        <v>372</v>
+      </c>
       <c r="AF175">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AG175">
         <v>125</v>
@@ -17616,7 +18702,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="176" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>528</v>
       </c>
@@ -17695,8 +18781,17 @@
       <c r="Z176">
         <v>50</v>
       </c>
+      <c r="AA176">
+        <v>20</v>
+      </c>
+      <c r="AB176">
+        <v>45</v>
+      </c>
+      <c r="AC176">
+        <v>413</v>
+      </c>
       <c r="AF176">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AG176">
         <v>128</v>
@@ -17711,7 +18806,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="177" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>530</v>
       </c>
@@ -17790,6 +18885,15 @@
       <c r="Z177">
         <v>10</v>
       </c>
+      <c r="AA177">
+        <v>20</v>
+      </c>
+      <c r="AB177">
+        <v>15</v>
+      </c>
+      <c r="AC177">
+        <v>60</v>
+      </c>
       <c r="AF177">
         <v>105</v>
       </c>
@@ -17806,7 +18910,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="178" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>531</v>
       </c>
@@ -17885,6 +18989,15 @@
       <c r="Z178">
         <v>5</v>
       </c>
+      <c r="AA178">
+        <v>20</v>
+      </c>
+      <c r="AB178">
+        <v>5</v>
+      </c>
+      <c r="AC178">
+        <v>40</v>
+      </c>
       <c r="AF178">
         <v>97</v>
       </c>
@@ -17901,7 +19014,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="179" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>532</v>
       </c>
@@ -17980,8 +19093,17 @@
       <c r="Z179">
         <v>40</v>
       </c>
+      <c r="AA179">
+        <v>20.5</v>
+      </c>
+      <c r="AB179">
+        <v>40</v>
+      </c>
+      <c r="AC179">
+        <v>283</v>
+      </c>
       <c r="AF179">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AG179">
         <v>18.5</v>
@@ -17996,7 +19118,7 @@
         <v>239.5</v>
       </c>
     </row>
-    <row r="180" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>536</v>
       </c>
@@ -18075,8 +19197,17 @@
       <c r="Z180">
         <v>45</v>
       </c>
+      <c r="AA180">
+        <v>20</v>
+      </c>
+      <c r="AB180">
+        <v>50</v>
+      </c>
+      <c r="AC180">
+        <v>487</v>
+      </c>
       <c r="AF180">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AG180">
         <v>123</v>
@@ -18091,7 +19222,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="181" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>537</v>
       </c>
@@ -18170,6 +19301,15 @@
       <c r="Z181">
         <v>10</v>
       </c>
+      <c r="AA181">
+        <v>20</v>
+      </c>
+      <c r="AB181">
+        <v>20</v>
+      </c>
+      <c r="AC181">
+        <v>80</v>
+      </c>
       <c r="AF181">
         <v>103</v>
       </c>
@@ -18186,7 +19326,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="182" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>538</v>
       </c>
@@ -18265,8 +19405,17 @@
       <c r="Z182">
         <v>35</v>
       </c>
+      <c r="AA182">
+        <v>20</v>
+      </c>
+      <c r="AB182">
+        <v>35</v>
+      </c>
+      <c r="AC182">
+        <v>233</v>
+      </c>
       <c r="AF182">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AG182">
         <v>119</v>
@@ -18281,7 +19430,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="183" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>543</v>
       </c>
@@ -18360,11 +19509,20 @@
       <c r="Z183">
         <v>45</v>
       </c>
+      <c r="AA183">
+        <v>27</v>
+      </c>
+      <c r="AB183">
+        <v>40</v>
+      </c>
+      <c r="AC183">
+        <v>510</v>
+      </c>
       <c r="AF183">
         <v>159</v>
       </c>
     </row>
-    <row r="184" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>550</v>
       </c>
@@ -18443,8 +19601,17 @@
       <c r="Z184">
         <v>40</v>
       </c>
+      <c r="AA184">
+        <v>15</v>
+      </c>
+      <c r="AB184">
+        <v>35</v>
+      </c>
+      <c r="AC184">
+        <v>273</v>
+      </c>
     </row>
-    <row r="185" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>549</v>
       </c>
@@ -18523,11 +19690,20 @@
       <c r="Z185">
         <v>15</v>
       </c>
+      <c r="AA185">
+        <v>20</v>
+      </c>
+      <c r="AB185">
+        <v>25</v>
+      </c>
+      <c r="AC185">
+        <v>120</v>
+      </c>
       <c r="AF185">
         <v>110</v>
       </c>
     </row>
-    <row r="186" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>551</v>
       </c>
@@ -18606,11 +19782,20 @@
       <c r="Z186">
         <v>35</v>
       </c>
+      <c r="AA186">
+        <v>22</v>
+      </c>
+      <c r="AB186">
+        <v>37</v>
+      </c>
+      <c r="AC186">
+        <v>377</v>
+      </c>
       <c r="AF186">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
-    <row r="187" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>552</v>
       </c>
@@ -18689,11 +19874,20 @@
       <c r="Z187">
         <v>25</v>
       </c>
+      <c r="AA187">
+        <v>25.5</v>
+      </c>
+      <c r="AB187">
+        <v>25</v>
+      </c>
+      <c r="AC187">
+        <v>276</v>
+      </c>
       <c r="AF187">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
-    <row r="188" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>561</v>
       </c>
@@ -18772,8 +19966,17 @@
       <c r="Z188">
         <v>10</v>
       </c>
+      <c r="AA188">
+        <v>22</v>
+      </c>
+      <c r="AB188">
+        <v>40</v>
+      </c>
+      <c r="AC188">
+        <v>413</v>
+      </c>
       <c r="AF188">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AG188">
         <v>122</v>
@@ -18788,99 +19991,9 @@
         <v>133</v>
       </c>
     </row>
-    <row r="189" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A189">
-        <v>562</v>
-      </c>
-      <c r="B189">
-        <v>21</v>
-      </c>
-      <c r="C189">
-        <v>20</v>
-      </c>
-      <c r="D189">
-        <v>0</v>
-      </c>
-      <c r="E189">
-        <v>10</v>
-      </c>
-      <c r="F189">
-        <v>0</v>
-      </c>
-      <c r="G189">
-        <v>5</v>
-      </c>
-      <c r="H189">
-        <v>0</v>
-      </c>
-      <c r="I189">
-        <v>0</v>
-      </c>
-      <c r="J189">
-        <v>0</v>
-      </c>
-      <c r="K189">
-        <v>10</v>
-      </c>
-      <c r="L189">
-        <v>5</v>
-      </c>
-      <c r="M189">
-        <v>15</v>
-      </c>
-      <c r="N189">
-        <v>10</v>
-      </c>
-      <c r="O189">
-        <v>0</v>
-      </c>
-      <c r="P189">
-        <v>0</v>
-      </c>
-      <c r="Q189">
-        <v>0</v>
-      </c>
-      <c r="R189">
-        <v>5</v>
-      </c>
-      <c r="S189">
-        <v>0</v>
-      </c>
-      <c r="T189">
-        <v>0</v>
-      </c>
-      <c r="U189">
-        <v>5</v>
-      </c>
-      <c r="V189">
-        <v>20</v>
-      </c>
-      <c r="W189">
-        <v>0</v>
-      </c>
-      <c r="X189">
-        <v>0</v>
-      </c>
-      <c r="Y189">
-        <v>20</v>
-      </c>
-      <c r="Z189">
-        <v>5</v>
-      </c>
+    <row r="189" spans="1:36" x14ac:dyDescent="0.3">
       <c r="AF189">
         <v>105</v>
-      </c>
-      <c r="AG189">
-        <v>98</v>
-      </c>
-      <c r="AH189">
-        <v>101</v>
-      </c>
-      <c r="AI189">
-        <v>107</v>
-      </c>
-      <c r="AJ189">
-        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Find best/worst ft nums, find corr MRI file names
</commit_message>
<xml_diff>
--- a/CRIq_new_dataworksheet.xlsx
+++ b/CRIq_new_dataworksheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\CRIq_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Thesis Work\CRIq_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="10212"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -512,9 +512,9 @@
       <selection sqref="A1:AJ189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +624,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>181</v>
       </c>
@@ -731,7 +731,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>182</v>
       </c>
@@ -835,7 +835,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>211</v>
       </c>
@@ -939,7 +939,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>212</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>213</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>214</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>215</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>216</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>217</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>218</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>241</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>242</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>243</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>244</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>245</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>246</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>247</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>248</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>249</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>250</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>251</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>253</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>254</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>255</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>256</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>257</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>258</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>61</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>62</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>63</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>64</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>65</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>66</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>67</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>68</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>69</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>70</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>71</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>72</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>91</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>92</v>
       </c>
@@ -4891,7 +4891,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>93</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>94</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>95</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>96</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>97</v>
       </c>
@@ -5411,7 +5411,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>98</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>99</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>421</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>422</v>
       </c>
@@ -5827,7 +5827,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>423</v>
       </c>
@@ -5931,7 +5931,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>424</v>
       </c>
@@ -6035,7 +6035,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>425</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>426</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>427</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1</v>
       </c>
@@ -6451,7 +6451,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2</v>
       </c>
@@ -6555,7 +6555,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>3</v>
       </c>
@@ -6659,7 +6659,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>5</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>6</v>
       </c>
@@ -6867,7 +6867,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>31</v>
       </c>
@@ -6965,7 +6965,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>32</v>
       </c>
@@ -7063,7 +7063,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>33</v>
       </c>
@@ -7167,7 +7167,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>34</v>
       </c>
@@ -7271,7 +7271,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>35</v>
       </c>
@@ -7375,7 +7375,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>36</v>
       </c>
@@ -7479,7 +7479,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>37</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>73</v>
       </c>
@@ -7675,7 +7675,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>331</v>
       </c>
@@ -7779,7 +7779,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>302</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>303</v>
       </c>
@@ -7987,7 +7987,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>364</v>
       </c>
@@ -8091,7 +8091,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>365</v>
       </c>
@@ -8195,7 +8195,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>366</v>
       </c>
@@ -8299,7 +8299,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>367</v>
       </c>
@@ -8403,7 +8403,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>368</v>
       </c>
@@ -8507,7 +8507,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>369</v>
       </c>
@@ -8611,7 +8611,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>370</v>
       </c>
@@ -8715,7 +8715,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>371</v>
       </c>
@@ -8819,7 +8819,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>372</v>
       </c>
@@ -8923,7 +8923,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>373</v>
       </c>
@@ -9027,7 +9027,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>374</v>
       </c>
@@ -9131,7 +9131,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>375</v>
       </c>
@@ -9235,7 +9235,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>376</v>
       </c>
@@ -9339,7 +9339,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="86" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>377</v>
       </c>
@@ -9443,7 +9443,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="87" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>378</v>
       </c>
@@ -9547,7 +9547,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="88" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>379</v>
       </c>
@@ -9651,7 +9651,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="89" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>271</v>
       </c>
@@ -9755,7 +9755,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="90" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>272</v>
       </c>
@@ -9859,7 +9859,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="91" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>273</v>
       </c>
@@ -9963,7 +9963,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="92" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>274</v>
       </c>
@@ -10067,7 +10067,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>275</v>
       </c>
@@ -10171,7 +10171,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="94" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>276</v>
       </c>
@@ -10275,7 +10275,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="95" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>277</v>
       </c>
@@ -10379,7 +10379,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="96" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>278</v>
       </c>
@@ -10483,7 +10483,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>279</v>
       </c>
@@ -10587,7 +10587,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="98" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>301</v>
       </c>
@@ -10691,7 +10691,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>302</v>
       </c>
@@ -10795,7 +10795,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="100" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>303</v>
       </c>
@@ -10899,7 +10899,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="101" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>304</v>
       </c>
@@ -11003,7 +11003,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="102" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>305</v>
       </c>
@@ -11107,7 +11107,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="103" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>306</v>
       </c>
@@ -11211,7 +11211,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="104" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>307</v>
       </c>
@@ -11315,7 +11315,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="105" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>308</v>
       </c>
@@ -11419,7 +11419,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="106" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>309</v>
       </c>
@@ -11523,7 +11523,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="107" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>310</v>
       </c>
@@ -11627,7 +11627,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="108" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>332</v>
       </c>
@@ -11731,7 +11731,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="109" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>333</v>
       </c>
@@ -11835,7 +11835,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="110" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>334</v>
       </c>
@@ -11939,7 +11939,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="111" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>335</v>
       </c>
@@ -12043,7 +12043,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="112" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>336</v>
       </c>
@@ -12147,7 +12147,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>337</v>
       </c>
@@ -12251,7 +12251,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>338</v>
       </c>
@@ -12355,7 +12355,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="115" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>339</v>
       </c>
@@ -12450,7 +12450,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="116" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>340</v>
       </c>
@@ -12554,7 +12554,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="117" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>533</v>
       </c>
@@ -12658,7 +12658,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="118" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>534</v>
       </c>
@@ -12762,7 +12762,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="119" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>535</v>
       </c>
@@ -12866,7 +12866,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>428</v>
       </c>
@@ -12970,7 +12970,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="121" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>429</v>
       </c>
@@ -13074,7 +13074,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="122" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>430</v>
       </c>
@@ -13178,7 +13178,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="123" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>403</v>
       </c>
@@ -13282,7 +13282,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="124" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>402</v>
       </c>
@@ -13386,7 +13386,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="125" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>401</v>
       </c>
@@ -13490,7 +13490,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="126" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>400</v>
       </c>
@@ -13594,7 +13594,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="127" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>399</v>
       </c>
@@ -13698,7 +13698,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="128" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>398</v>
       </c>
@@ -13802,7 +13802,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="129" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>391</v>
       </c>
@@ -13906,7 +13906,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="130" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>397</v>
       </c>
@@ -14010,7 +14010,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="131" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>396</v>
       </c>
@@ -14114,7 +14114,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="132" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>395</v>
       </c>
@@ -14218,7 +14218,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="133" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>394</v>
       </c>
@@ -14322,7 +14322,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="134" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>393</v>
       </c>
@@ -14426,7 +14426,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="135" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>392</v>
       </c>
@@ -14530,7 +14530,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="136" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>526</v>
       </c>
@@ -14634,7 +14634,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="137" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>539</v>
       </c>
@@ -14738,7 +14738,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="138" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>540</v>
       </c>
@@ -14842,7 +14842,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="139" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>542</v>
       </c>
@@ -14946,7 +14946,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="140" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>545</v>
       </c>
@@ -15050,7 +15050,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>548</v>
       </c>
@@ -15154,7 +15154,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="142" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>560</v>
       </c>
@@ -15258,7 +15258,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="143" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>570</v>
       </c>
@@ -15362,7 +15362,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="144" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>571</v>
       </c>
@@ -15466,7 +15466,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="145" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>573</v>
       </c>
@@ -15570,7 +15570,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="146" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>575</v>
       </c>
@@ -15674,7 +15674,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="147" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>451</v>
       </c>
@@ -15778,7 +15778,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="148" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>452</v>
       </c>
@@ -15882,7 +15882,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="149" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>453</v>
       </c>
@@ -15986,7 +15986,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="150" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>454</v>
       </c>
@@ -16090,7 +16090,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="151" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>455</v>
       </c>
@@ -16194,7 +16194,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="152" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>456</v>
       </c>
@@ -16298,7 +16298,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="153" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>457</v>
       </c>
@@ -16402,7 +16402,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="154" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>458</v>
       </c>
@@ -16506,7 +16506,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="155" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>459</v>
       </c>
@@ -16610,7 +16610,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="156" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>460</v>
       </c>
@@ -16714,7 +16714,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="157" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>461</v>
       </c>
@@ -16818,7 +16818,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="158" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>462</v>
       </c>
@@ -16922,7 +16922,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="159" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>481</v>
       </c>
@@ -17026,7 +17026,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="160" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>121</v>
       </c>
@@ -17130,7 +17130,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="161" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>122</v>
       </c>
@@ -17234,7 +17234,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="162" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>123</v>
       </c>
@@ -17338,7 +17338,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="163" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>124</v>
       </c>
@@ -17442,7 +17442,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="164" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>125</v>
       </c>
@@ -17546,7 +17546,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="165" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>151</v>
       </c>
@@ -17650,7 +17650,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="166" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>152</v>
       </c>
@@ -17754,7 +17754,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="167" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>153</v>
       </c>
@@ -17858,7 +17858,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="168" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>100</v>
       </c>
@@ -17962,7 +17962,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="169" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>101</v>
       </c>
@@ -18066,7 +18066,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="170" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>426</v>
       </c>
@@ -18170,7 +18170,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="171" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>500</v>
       </c>
@@ -18274,7 +18274,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="172" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>520</v>
       </c>
@@ -18378,7 +18378,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="173" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>521</v>
       </c>
@@ -18482,7 +18482,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="174" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>525</v>
       </c>
@@ -18586,7 +18586,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="175" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>527</v>
       </c>
@@ -18690,7 +18690,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="176" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>528</v>
       </c>
@@ -18794,7 +18794,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="177" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>530</v>
       </c>
@@ -18898,7 +18898,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="178" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>531</v>
       </c>
@@ -19002,7 +19002,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="179" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>532</v>
       </c>
@@ -19106,7 +19106,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="180" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>536</v>
       </c>
@@ -19210,7 +19210,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="181" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>537</v>
       </c>
@@ -19314,7 +19314,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="182" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>538</v>
       </c>
@@ -19418,7 +19418,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="183" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>543</v>
       </c>
@@ -19519,7 +19519,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="184" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>550</v>
       </c>
@@ -19608,7 +19608,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="185" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>549</v>
       </c>
@@ -19709,7 +19709,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="186" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>551</v>
       </c>
@@ -19810,7 +19810,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="187" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>552</v>
       </c>
@@ -19911,7 +19911,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="188" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>561</v>
       </c>
@@ -20015,7 +20015,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="189" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AF189">
         <v>105</v>
       </c>

</xml_diff>